<commit_message>
Updated data in endo-learn/BGSaWC to IEA World Energy Outlook 2019; corrected reference text in About tab of elec/BCRbQ
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/BGSaWC/BAU Global Solar and Wind Cap.xlsx
+++ b/InputData/endo-learn/BGSaWC/BAU Global Solar and Wind Cap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\endo-learn\BGSaWC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\endo-learn\BGSaWC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Wind_Capacity" sheetId="2" r:id="rId2"/>
-    <sheet name="Solar_Capacity" sheetId="3" r:id="rId3"/>
-    <sheet name="BGSaWC" sheetId="4" r:id="rId4"/>
+    <sheet name="IEA 2019 outlook" sheetId="5" r:id="rId2"/>
+    <sheet name="IEA 2017 Wind" sheetId="2" r:id="rId3"/>
+    <sheet name="IEA 2017 Solar" sheetId="3" r:id="rId4"/>
+    <sheet name="BGSaWC" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>BGSaWC BAU Global Solar and Wind Capacities</t>
   </si>
@@ -87,9 +88,6 @@
   </si>
   <si>
     <t>Reference Technology Scenario (RTS)</t>
-  </si>
-  <si>
-    <t>Main Source</t>
   </si>
   <si>
     <t>Alternate Source (not presently used)</t>
@@ -166,6 +164,36 @@
   <si>
     <t>Global Capacity (MW)</t>
   </si>
+  <si>
+    <t>Data manually extra from website</t>
+  </si>
+  <si>
+    <t>https://www.iea.org/weo2019/</t>
+  </si>
+  <si>
+    <t>World Energy Outlook</t>
+  </si>
+  <si>
+    <t>Year over year trend in IEA 2017 Data, 2040-2050</t>
+  </si>
+  <si>
+    <t>Solar Capacity</t>
+  </si>
+  <si>
+    <t>Wind Capacity</t>
+  </si>
+  <si>
+    <t>Interactive graph: Installed power generation capacity in the Stated Policies Scenario</t>
+  </si>
+  <si>
+    <t>Solar and Onshore Wind, 2017-2040</t>
+  </si>
+  <si>
+    <t>Year over year growth for solar and onshore wind, 2040-2050; Offshore wind</t>
+  </si>
+  <si>
+    <t>Onshore Wind</t>
+  </si>
 </sst>
 </file>
 
@@ -177,7 +205,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0;\-#,##0;_(* &quot; - &quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +277,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -302,7 +336,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -339,6 +373,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1615,101 +1664,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="12">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B10" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>2017</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B13" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="12">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1717,25 +1799,821 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B2" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2019</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2021</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2022</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2023</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2024</v>
+      </c>
+      <c r="J2" s="5">
+        <v>2025</v>
+      </c>
+      <c r="K2" s="5">
+        <v>2026</v>
+      </c>
+      <c r="L2" s="5">
+        <v>2027</v>
+      </c>
+      <c r="M2" s="5">
+        <v>2028</v>
+      </c>
+      <c r="N2" s="5">
+        <v>2029</v>
+      </c>
+      <c r="O2" s="5">
+        <v>2030</v>
+      </c>
+      <c r="P2" s="5">
+        <v>2031</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>2032</v>
+      </c>
+      <c r="R2" s="5">
+        <v>2033</v>
+      </c>
+      <c r="S2" s="5">
+        <v>2034</v>
+      </c>
+      <c r="T2" s="5">
+        <v>2035</v>
+      </c>
+      <c r="U2" s="5">
+        <v>2036</v>
+      </c>
+      <c r="V2" s="5">
+        <v>2037</v>
+      </c>
+      <c r="W2" s="5">
+        <v>2038</v>
+      </c>
+      <c r="X2" s="5">
+        <v>2039</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>2040</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>2041</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>2042</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>2043</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>2044</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>2045</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>2046</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>2047</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>2048</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>2049</v>
+      </c>
+      <c r="AI2" s="5">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>399</v>
+      </c>
+      <c r="C3">
+        <v>495</v>
+      </c>
+      <c r="D3">
+        <v>607</v>
+      </c>
+      <c r="E3">
+        <v>715</v>
+      </c>
+      <c r="F3">
+        <v>825</v>
+      </c>
+      <c r="G3">
+        <v>943</v>
+      </c>
+      <c r="H3">
+        <v>1070</v>
+      </c>
+      <c r="I3">
+        <v>1202</v>
+      </c>
+      <c r="J3">
+        <v>1309</v>
+      </c>
+      <c r="K3">
+        <v>1415</v>
+      </c>
+      <c r="L3">
+        <v>1522</v>
+      </c>
+      <c r="M3">
+        <v>1631</v>
+      </c>
+      <c r="N3">
+        <v>1746</v>
+      </c>
+      <c r="O3">
+        <v>1866</v>
+      </c>
+      <c r="P3">
+        <v>1985</v>
+      </c>
+      <c r="Q3">
+        <v>2104</v>
+      </c>
+      <c r="R3">
+        <v>2225</v>
+      </c>
+      <c r="S3">
+        <v>2349</v>
+      </c>
+      <c r="T3">
+        <v>2476</v>
+      </c>
+      <c r="U3">
+        <v>2606</v>
+      </c>
+      <c r="V3">
+        <v>2738</v>
+      </c>
+      <c r="W3">
+        <v>2872</v>
+      </c>
+      <c r="X3">
+        <v>3007</v>
+      </c>
+      <c r="Y3">
+        <v>3142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z4">
+        <f>'IEA 2017 Solar'!AE12/'IEA 2017 Solar'!$AD$12</f>
+        <v>1.0413981483651269</v>
+      </c>
+      <c r="AA4">
+        <f>'IEA 2017 Solar'!AF12/'IEA 2017 Solar'!$AD$12</f>
+        <v>1.0827962967302536</v>
+      </c>
+      <c r="AB4">
+        <f>'IEA 2017 Solar'!AG12/'IEA 2017 Solar'!$AD$12</f>
+        <v>1.1241944450953805</v>
+      </c>
+      <c r="AC4">
+        <f>'IEA 2017 Solar'!AH12/'IEA 2017 Solar'!$AD$12</f>
+        <v>1.1655925934605074</v>
+      </c>
+      <c r="AD4">
+        <f>'IEA 2017 Solar'!AI12/'IEA 2017 Solar'!$AD$12</f>
+        <v>1.2069907418256338</v>
+      </c>
+      <c r="AE4">
+        <f>'IEA 2017 Solar'!AJ12/'IEA 2017 Solar'!$AD$12</f>
+        <v>1.2512680731867143</v>
+      </c>
+      <c r="AF4">
+        <f>'IEA 2017 Solar'!AK12/'IEA 2017 Solar'!$AD$12</f>
+        <v>1.2955454045477948</v>
+      </c>
+      <c r="AG4">
+        <f>'IEA 2017 Solar'!AL12/'IEA 2017 Solar'!$AD$12</f>
+        <v>1.3398227359088752</v>
+      </c>
+      <c r="AH4">
+        <f>'IEA 2017 Solar'!AM12/'IEA 2017 Solar'!$AD$12</f>
+        <v>1.3841000672699557</v>
+      </c>
+      <c r="AI4">
+        <f>'IEA 2017 Solar'!AN12/'IEA 2017 Solar'!$AD$12</f>
+        <v>1.4283773986310362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="19">
+        <f>B3</f>
+        <v>399</v>
+      </c>
+      <c r="C5" s="19">
+        <f>C3</f>
+        <v>495</v>
+      </c>
+      <c r="D5" s="19">
+        <f>D3</f>
+        <v>607</v>
+      </c>
+      <c r="E5" s="19">
+        <f>E3</f>
+        <v>715</v>
+      </c>
+      <c r="F5" s="19">
+        <f>F3</f>
+        <v>825</v>
+      </c>
+      <c r="G5" s="19">
+        <f>G3</f>
+        <v>943</v>
+      </c>
+      <c r="H5" s="19">
+        <f>H3</f>
+        <v>1070</v>
+      </c>
+      <c r="I5" s="19">
+        <f>I3</f>
+        <v>1202</v>
+      </c>
+      <c r="J5" s="19">
+        <f>J3</f>
+        <v>1309</v>
+      </c>
+      <c r="K5" s="19">
+        <f>K3</f>
+        <v>1415</v>
+      </c>
+      <c r="L5" s="19">
+        <f>L3</f>
+        <v>1522</v>
+      </c>
+      <c r="M5" s="19">
+        <f>M3</f>
+        <v>1631</v>
+      </c>
+      <c r="N5" s="19">
+        <f>N3</f>
+        <v>1746</v>
+      </c>
+      <c r="O5" s="19">
+        <f>O3</f>
+        <v>1866</v>
+      </c>
+      <c r="P5" s="19">
+        <f>P3</f>
+        <v>1985</v>
+      </c>
+      <c r="Q5" s="19">
+        <f>Q3</f>
+        <v>2104</v>
+      </c>
+      <c r="R5" s="19">
+        <f>R3</f>
+        <v>2225</v>
+      </c>
+      <c r="S5" s="19">
+        <f>S3</f>
+        <v>2349</v>
+      </c>
+      <c r="T5" s="19">
+        <f>T3</f>
+        <v>2476</v>
+      </c>
+      <c r="U5" s="19">
+        <f>U3</f>
+        <v>2606</v>
+      </c>
+      <c r="V5" s="19">
+        <f>V3</f>
+        <v>2738</v>
+      </c>
+      <c r="W5" s="19">
+        <f>W3</f>
+        <v>2872</v>
+      </c>
+      <c r="X5" s="19">
+        <f>X3</f>
+        <v>3007</v>
+      </c>
+      <c r="Y5" s="19">
+        <f>Y3</f>
+        <v>3142</v>
+      </c>
+      <c r="Z5" s="19">
+        <f>$Y$5*Z4</f>
+        <v>3272.0729821632285</v>
+      </c>
+      <c r="AA5" s="19">
+        <f>$Y$5*AA4</f>
+        <v>3402.1459643264566</v>
+      </c>
+      <c r="AB5" s="19">
+        <f>$Y$5*AB4</f>
+        <v>3532.2189464896855</v>
+      </c>
+      <c r="AC5" s="19">
+        <f>$Y$5*AC4</f>
+        <v>3662.2919286529141</v>
+      </c>
+      <c r="AD5" s="19">
+        <f>$Y$5*AD4</f>
+        <v>3792.3649108161417</v>
+      </c>
+      <c r="AE5" s="19">
+        <f>$Y$5*AE4</f>
+        <v>3931.4842859526561</v>
+      </c>
+      <c r="AF5" s="19">
+        <f>$Y$5*AF4</f>
+        <v>4070.6036610891711</v>
+      </c>
+      <c r="AG5" s="19">
+        <f>$Y$5*AG4</f>
+        <v>4209.723036225686</v>
+      </c>
+      <c r="AH5" s="19">
+        <f>$Y$5*AH4</f>
+        <v>4348.8424113622004</v>
+      </c>
+      <c r="AI5" s="19">
+        <f>$Y$5*AI4</f>
+        <v>4487.9617864987158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2019</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2021</v>
+      </c>
+      <c r="G8" s="5">
+        <v>2022</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2023</v>
+      </c>
+      <c r="I8" s="5">
+        <v>2024</v>
+      </c>
+      <c r="J8" s="5">
+        <v>2025</v>
+      </c>
+      <c r="K8" s="5">
+        <v>2026</v>
+      </c>
+      <c r="L8" s="5">
+        <v>2027</v>
+      </c>
+      <c r="M8" s="5">
+        <v>2028</v>
+      </c>
+      <c r="N8" s="5">
+        <v>2029</v>
+      </c>
+      <c r="O8" s="5">
+        <v>2030</v>
+      </c>
+      <c r="P8" s="5">
+        <v>2031</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>2032</v>
+      </c>
+      <c r="R8" s="5">
+        <v>2033</v>
+      </c>
+      <c r="S8" s="5">
+        <v>2034</v>
+      </c>
+      <c r="T8" s="5">
+        <v>2035</v>
+      </c>
+      <c r="U8" s="5">
+        <v>2036</v>
+      </c>
+      <c r="V8" s="5">
+        <v>2037</v>
+      </c>
+      <c r="W8" s="5">
+        <v>2038</v>
+      </c>
+      <c r="X8" s="5">
+        <v>2039</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>2040</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>2041</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>2042</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>2043</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>2044</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>2045</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>2046</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>2047</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>2048</v>
+      </c>
+      <c r="AH8" s="5">
+        <v>2049</v>
+      </c>
+      <c r="AI8" s="5">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>515</v>
+      </c>
+      <c r="C9">
+        <v>566</v>
+      </c>
+      <c r="D9">
+        <v>624</v>
+      </c>
+      <c r="E9">
+        <v>688</v>
+      </c>
+      <c r="F9">
+        <v>747</v>
+      </c>
+      <c r="G9">
+        <v>804</v>
+      </c>
+      <c r="H9">
+        <v>861</v>
+      </c>
+      <c r="I9">
+        <v>921</v>
+      </c>
+      <c r="J9">
+        <v>980</v>
+      </c>
+      <c r="K9">
+        <v>1040</v>
+      </c>
+      <c r="L9">
+        <v>1100</v>
+      </c>
+      <c r="M9">
+        <v>1162</v>
+      </c>
+      <c r="N9">
+        <v>1224</v>
+      </c>
+      <c r="O9">
+        <v>1288</v>
+      </c>
+      <c r="P9">
+        <v>1352</v>
+      </c>
+      <c r="Q9">
+        <v>1415</v>
+      </c>
+      <c r="R9">
+        <v>1476</v>
+      </c>
+      <c r="S9">
+        <v>1536</v>
+      </c>
+      <c r="T9">
+        <v>1594</v>
+      </c>
+      <c r="U9">
+        <v>1649</v>
+      </c>
+      <c r="V9">
+        <v>1703</v>
+      </c>
+      <c r="W9">
+        <v>1754</v>
+      </c>
+      <c r="X9">
+        <v>1806</v>
+      </c>
+      <c r="Y9">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z10">
+        <f>'IEA 2017 Wind'!AE9/'IEA 2017 Wind'!$AD$9</f>
+        <v>1.0207393875977682</v>
+      </c>
+      <c r="AA10">
+        <f>'IEA 2017 Wind'!AF9/'IEA 2017 Wind'!$AD$9</f>
+        <v>1.0414787751955361</v>
+      </c>
+      <c r="AB10">
+        <f>'IEA 2017 Wind'!AG9/'IEA 2017 Wind'!$AD$9</f>
+        <v>1.0622181627933043</v>
+      </c>
+      <c r="AC10">
+        <f>'IEA 2017 Wind'!AH9/'IEA 2017 Wind'!$AD$9</f>
+        <v>1.0829575503910722</v>
+      </c>
+      <c r="AD10">
+        <f>'IEA 2017 Wind'!AI9/'IEA 2017 Wind'!$AD$9</f>
+        <v>1.1036969379888402</v>
+      </c>
+      <c r="AE10">
+        <f>'IEA 2017 Wind'!AJ9/'IEA 2017 Wind'!$AD$9</f>
+        <v>1.135431778422568</v>
+      </c>
+      <c r="AF10">
+        <f>'IEA 2017 Wind'!AK9/'IEA 2017 Wind'!$AD$9</f>
+        <v>1.1671666188562957</v>
+      </c>
+      <c r="AG10">
+        <f>'IEA 2017 Wind'!AL9/'IEA 2017 Wind'!$AD$9</f>
+        <v>1.1989014592900236</v>
+      </c>
+      <c r="AH10">
+        <f>'IEA 2017 Wind'!AM9/'IEA 2017 Wind'!$AD$9</f>
+        <v>1.2306362997237512</v>
+      </c>
+      <c r="AI10">
+        <f>'IEA 2017 Wind'!AN9/'IEA 2017 Wind'!$AD$9</f>
+        <v>1.2623711401574789</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ref="B11:X11" si="0">B9</f>
+        <v>515</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>566</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>624</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>688</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>747</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>804</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>861</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>921</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>980</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>1040</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>1162</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>1224</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>1288</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>1352</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>1415</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>1476</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>1536</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>1594</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="0"/>
+        <v>1649</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="0"/>
+        <v>1703</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="0"/>
+        <v>1754</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="0"/>
+        <v>1806</v>
+      </c>
+      <c r="Y11">
+        <f>Y9</f>
+        <v>1856</v>
+      </c>
+      <c r="Z11">
+        <f>$Y$9*Z10</f>
+        <v>1894.4923033814578</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" ref="AA11:AI11" si="1">$Y$9*AA10</f>
+        <v>1932.9846067629151</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="1"/>
+        <v>1971.4769101443728</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="1"/>
+        <v>2009.9692135258301</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="1"/>
+        <v>2048.4615169072872</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="1"/>
+        <v>2107.3613807522861</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="1"/>
+        <v>2166.261244597285</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="1"/>
+        <v>2225.1611084422839</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="1"/>
+        <v>2284.0609722872823</v>
+      </c>
+      <c r="AI11">
+        <f t="shared" si="1"/>
+        <v>2342.9608361322807</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:AN22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="AN10" sqref="AN10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="38" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="38" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:40" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:40" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1857,7 +2735,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -2003,7 +2881,7 @@
         <v>2072.8400198583167</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -2149,12 +3027,12 @@
         <v>135.57703324231764</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -2246,7 +3124,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>8</v>
       </c>
@@ -2338,7 +3216,7 @@
         <v>1977.5444351764106</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>9</v>
       </c>
@@ -2446,32 +3324,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A9:AN25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="Q7" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:40" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:40" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2593,7 +3471,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
@@ -2739,7 +3617,7 @@
         <v>2396.4039058194176</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
@@ -2885,7 +3763,7 @@
         <v>217.01252172511622</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -2977,7 +3855,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>13</v>
       </c>
@@ -3069,7 +3947,7 @@
         <v>3112.2072054934733</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>14</v>
       </c>
@@ -3161,7 +4039,7 @@
         <v>1387.1410874692133</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>15</v>
       </c>
@@ -3279,7 +4157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -3287,17 +4165,18 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14:AI14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.3984375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -3402,1716 +4281,1716 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A3" s="16" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A4" s="16" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A5" s="16" t="s">
+      <c r="B6" s="17">
+        <f>'IEA 2019 outlook'!B11*10^3</f>
+        <v>515000</v>
+      </c>
+      <c r="C6" s="17">
+        <f>'IEA 2019 outlook'!C11*10^3</f>
+        <v>566000</v>
+      </c>
+      <c r="D6" s="17">
+        <f>'IEA 2019 outlook'!D11*10^3</f>
+        <v>624000</v>
+      </c>
+      <c r="E6" s="17">
+        <f>'IEA 2019 outlook'!E11*10^3</f>
+        <v>688000</v>
+      </c>
+      <c r="F6" s="17">
+        <f>'IEA 2019 outlook'!F11*10^3</f>
+        <v>747000</v>
+      </c>
+      <c r="G6" s="17">
+        <f>'IEA 2019 outlook'!G11*10^3</f>
+        <v>804000</v>
+      </c>
+      <c r="H6" s="17">
+        <f>'IEA 2019 outlook'!H11*10^3</f>
+        <v>861000</v>
+      </c>
+      <c r="I6" s="17">
+        <f>'IEA 2019 outlook'!I11*10^3</f>
+        <v>921000</v>
+      </c>
+      <c r="J6" s="17">
+        <f>'IEA 2019 outlook'!J11*10^3</f>
+        <v>980000</v>
+      </c>
+      <c r="K6" s="17">
+        <f>'IEA 2019 outlook'!K11*10^3</f>
+        <v>1040000</v>
+      </c>
+      <c r="L6" s="17">
+        <f>'IEA 2019 outlook'!L11*10^3</f>
+        <v>1100000</v>
+      </c>
+      <c r="M6" s="17">
+        <f>'IEA 2019 outlook'!M11*10^3</f>
+        <v>1162000</v>
+      </c>
+      <c r="N6" s="17">
+        <f>'IEA 2019 outlook'!N11*10^3</f>
+        <v>1224000</v>
+      </c>
+      <c r="O6" s="17">
+        <f>'IEA 2019 outlook'!O11*10^3</f>
+        <v>1288000</v>
+      </c>
+      <c r="P6" s="17">
+        <f>'IEA 2019 outlook'!P11*10^3</f>
+        <v>1352000</v>
+      </c>
+      <c r="Q6" s="17">
+        <f>'IEA 2019 outlook'!Q11*10^3</f>
+        <v>1415000</v>
+      </c>
+      <c r="R6" s="17">
+        <f>'IEA 2019 outlook'!R11*10^3</f>
+        <v>1476000</v>
+      </c>
+      <c r="S6" s="17">
+        <f>'IEA 2019 outlook'!S11*10^3</f>
+        <v>1536000</v>
+      </c>
+      <c r="T6" s="17">
+        <f>'IEA 2019 outlook'!T11*10^3</f>
+        <v>1594000</v>
+      </c>
+      <c r="U6" s="17">
+        <f>'IEA 2019 outlook'!U11*10^3</f>
+        <v>1649000</v>
+      </c>
+      <c r="V6" s="17">
+        <f>'IEA 2019 outlook'!V11*10^3</f>
+        <v>1703000</v>
+      </c>
+      <c r="W6" s="17">
+        <f>'IEA 2019 outlook'!W11*10^3</f>
+        <v>1754000</v>
+      </c>
+      <c r="X6" s="17">
+        <f>'IEA 2019 outlook'!X11*10^3</f>
+        <v>1806000</v>
+      </c>
+      <c r="Y6" s="17">
+        <f>'IEA 2019 outlook'!Y11*10^3</f>
+        <v>1856000</v>
+      </c>
+      <c r="Z6" s="17">
+        <f>'IEA 2019 outlook'!Z11*10^3</f>
+        <v>1894492.3033814577</v>
+      </c>
+      <c r="AA6" s="17">
+        <f>'IEA 2019 outlook'!AA11*10^3</f>
+        <v>1932984.6067629152</v>
+      </c>
+      <c r="AB6" s="17">
+        <f>'IEA 2019 outlook'!AB11*10^3</f>
+        <v>1971476.9101443728</v>
+      </c>
+      <c r="AC6" s="17">
+        <f>'IEA 2019 outlook'!AC11*10^3</f>
+        <v>2009969.2135258301</v>
+      </c>
+      <c r="AD6" s="17">
+        <f>'IEA 2019 outlook'!AD11*10^3</f>
+        <v>2048461.5169072873</v>
+      </c>
+      <c r="AE6" s="17">
+        <f>'IEA 2019 outlook'!AE11*10^3</f>
+        <v>2107361.3807522859</v>
+      </c>
+      <c r="AF6" s="17">
+        <f>'IEA 2019 outlook'!AF11*10^3</f>
+        <v>2166261.2445972851</v>
+      </c>
+      <c r="AG6" s="17">
+        <f>'IEA 2019 outlook'!AG11*10^3</f>
+        <v>2225161.1084422837</v>
+      </c>
+      <c r="AH6" s="17">
+        <f>'IEA 2019 outlook'!AH11*10^3</f>
+        <v>2284060.9722872823</v>
+      </c>
+      <c r="AI6" s="17">
+        <f>'IEA 2019 outlook'!AI11*10^3</f>
+        <v>2342960.8361322805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
-      <c r="AG5">
-        <v>0</v>
-      </c>
-      <c r="AH5">
-        <v>0</v>
-      </c>
-      <c r="AI5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="17">
-        <f>Wind_Capacity!G9*10^3</f>
-        <v>507658.45341373654</v>
-      </c>
-      <c r="C6" s="17">
-        <f>Wind_Capacity!H9*10^3</f>
-        <v>563276.28609345283</v>
-      </c>
-      <c r="D6" s="17">
-        <f>Wind_Capacity!I9*10^3</f>
-        <v>618894.11877316923</v>
-      </c>
-      <c r="E6" s="17">
-        <f>Wind_Capacity!J9*10^3</f>
-        <v>674511.95145288552</v>
-      </c>
-      <c r="F6" s="17">
-        <f>Wind_Capacity!K9*10^3</f>
-        <v>730129.78413260193</v>
-      </c>
-      <c r="G6" s="17">
-        <f>Wind_Capacity!L9*10^3</f>
-        <v>785747.61681231821</v>
-      </c>
-      <c r="H6" s="17">
-        <f>Wind_Capacity!M9*10^3</f>
-        <v>841365.44949203462</v>
-      </c>
-      <c r="I6" s="17">
-        <f>Wind_Capacity!N9*10^3</f>
-        <v>896983.28217175091</v>
-      </c>
-      <c r="J6" s="17">
-        <f>Wind_Capacity!O9*10^3</f>
-        <v>952601.11485146743</v>
-      </c>
-      <c r="K6" s="17">
-        <f>Wind_Capacity!P9*10^3</f>
-        <v>1005542.291022492</v>
-      </c>
-      <c r="L6" s="17">
-        <f>Wind_Capacity!Q9*10^3</f>
-        <v>1058483.4671935167</v>
-      </c>
-      <c r="M6" s="17">
-        <f>Wind_Capacity!R9*10^3</f>
-        <v>1111424.6433645412</v>
-      </c>
-      <c r="N6" s="17">
-        <f>Wind_Capacity!S9*10^3</f>
-        <v>1164365.8195355658</v>
-      </c>
-      <c r="O6" s="17">
-        <f>Wind_Capacity!T9*10^3</f>
-        <v>1217306.9957065906</v>
-      </c>
-      <c r="P6" s="17">
-        <f>Wind_Capacity!U9*10^3</f>
-        <v>1265276.7832629781</v>
-      </c>
-      <c r="Q6" s="17">
-        <f>Wind_Capacity!V9*10^3</f>
-        <v>1313246.5708193656</v>
-      </c>
-      <c r="R6" s="17">
-        <f>Wind_Capacity!W9*10^3</f>
-        <v>1361216.358375753</v>
-      </c>
-      <c r="S6" s="17">
-        <f>Wind_Capacity!X9*10^3</f>
-        <v>1409186.1459321405</v>
-      </c>
-      <c r="T6" s="17">
-        <f>Wind_Capacity!Y9*10^3</f>
-        <v>1457155.9334885282</v>
-      </c>
-      <c r="U6" s="17">
-        <f>Wind_Capacity!Z9*10^3</f>
-        <v>1494128.9623054031</v>
-      </c>
-      <c r="V6" s="17">
-        <f>Wind_Capacity!AA9*10^3</f>
-        <v>1531101.9911222779</v>
-      </c>
-      <c r="W6" s="17">
-        <f>Wind_Capacity!AB9*10^3</f>
-        <v>1568075.0199391528</v>
-      </c>
-      <c r="X6" s="17">
-        <f>Wind_Capacity!AC9*10^3</f>
-        <v>1605048.0487560276</v>
-      </c>
-      <c r="Y6" s="17">
-        <f>Wind_Capacity!AD9*10^3</f>
-        <v>1642021.0775729024</v>
-      </c>
-      <c r="Z6" s="17">
-        <f>Wind_Capacity!AE9*10^3</f>
-        <v>1676075.5891443917</v>
-      </c>
-      <c r="AA6" s="17">
-        <f>Wind_Capacity!AF9*10^3</f>
-        <v>1710130.100715881</v>
-      </c>
-      <c r="AB6" s="17">
-        <f>Wind_Capacity!AG9*10^3</f>
-        <v>1744184.61228737</v>
-      </c>
-      <c r="AC6" s="17">
-        <f>Wind_Capacity!AH9*10^3</f>
-        <v>1778239.1238588593</v>
-      </c>
-      <c r="AD6" s="17">
-        <f>Wind_Capacity!AI9*10^3</f>
-        <v>1812293.6354303483</v>
-      </c>
-      <c r="AE6" s="17">
-        <f>Wind_Capacity!AJ9*10^3</f>
-        <v>1864402.9123159421</v>
-      </c>
-      <c r="AF6" s="17">
-        <f>Wind_Capacity!AK9*10^3</f>
-        <v>1916512.1892015359</v>
-      </c>
-      <c r="AG6" s="17">
-        <f>Wind_Capacity!AL9*10^3</f>
-        <v>1968621.4660871297</v>
-      </c>
-      <c r="AH6" s="17">
-        <f>Wind_Capacity!AM9*10^3</f>
-        <v>2020730.7429727234</v>
-      </c>
-      <c r="AI6" s="17">
-        <f>Wind_Capacity!AN9*10^3</f>
-        <v>2072840.0198583168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A7" s="16" t="s">
+      <c r="B7" s="17">
+        <f>'IEA 2019 outlook'!B5*10^3</f>
+        <v>399000</v>
+      </c>
+      <c r="C7" s="17">
+        <f>'IEA 2019 outlook'!C5*10^3</f>
+        <v>495000</v>
+      </c>
+      <c r="D7" s="17">
+        <f>'IEA 2019 outlook'!D5*10^3</f>
+        <v>607000</v>
+      </c>
+      <c r="E7" s="17">
+        <f>'IEA 2019 outlook'!E5*10^3</f>
+        <v>715000</v>
+      </c>
+      <c r="F7" s="17">
+        <f>'IEA 2019 outlook'!F5*10^3</f>
+        <v>825000</v>
+      </c>
+      <c r="G7" s="17">
+        <f>'IEA 2019 outlook'!G5*10^3</f>
+        <v>943000</v>
+      </c>
+      <c r="H7" s="17">
+        <f>'IEA 2019 outlook'!H5*10^3</f>
+        <v>1070000</v>
+      </c>
+      <c r="I7" s="17">
+        <f>'IEA 2019 outlook'!I5*10^3</f>
+        <v>1202000</v>
+      </c>
+      <c r="J7" s="17">
+        <f>'IEA 2019 outlook'!J5*10^3</f>
+        <v>1309000</v>
+      </c>
+      <c r="K7" s="17">
+        <f>'IEA 2019 outlook'!K5*10^3</f>
+        <v>1415000</v>
+      </c>
+      <c r="L7" s="17">
+        <f>'IEA 2019 outlook'!L5*10^3</f>
+        <v>1522000</v>
+      </c>
+      <c r="M7" s="17">
+        <f>'IEA 2019 outlook'!M5*10^3</f>
+        <v>1631000</v>
+      </c>
+      <c r="N7" s="17">
+        <f>'IEA 2019 outlook'!N5*10^3</f>
+        <v>1746000</v>
+      </c>
+      <c r="O7" s="17">
+        <f>'IEA 2019 outlook'!O5*10^3</f>
+        <v>1866000</v>
+      </c>
+      <c r="P7" s="17">
+        <f>'IEA 2019 outlook'!P5*10^3</f>
+        <v>1985000</v>
+      </c>
+      <c r="Q7" s="17">
+        <f>'IEA 2019 outlook'!Q5*10^3</f>
+        <v>2104000</v>
+      </c>
+      <c r="R7" s="17">
+        <f>'IEA 2019 outlook'!R5*10^3</f>
+        <v>2225000</v>
+      </c>
+      <c r="S7" s="17">
+        <f>'IEA 2019 outlook'!S5*10^3</f>
+        <v>2349000</v>
+      </c>
+      <c r="T7" s="17">
+        <f>'IEA 2019 outlook'!T5*10^3</f>
+        <v>2476000</v>
+      </c>
+      <c r="U7" s="17">
+        <f>'IEA 2019 outlook'!U5*10^3</f>
+        <v>2606000</v>
+      </c>
+      <c r="V7" s="17">
+        <f>'IEA 2019 outlook'!V5*10^3</f>
+        <v>2738000</v>
+      </c>
+      <c r="W7" s="17">
+        <f>'IEA 2019 outlook'!W5*10^3</f>
+        <v>2872000</v>
+      </c>
+      <c r="X7" s="17">
+        <f>'IEA 2019 outlook'!X5*10^3</f>
+        <v>3007000</v>
+      </c>
+      <c r="Y7" s="17">
+        <f>'IEA 2019 outlook'!Y5*10^3</f>
+        <v>3142000</v>
+      </c>
+      <c r="Z7" s="17">
+        <f>'IEA 2019 outlook'!Z5*10^3</f>
+        <v>3272072.9821632286</v>
+      </c>
+      <c r="AA7" s="17">
+        <f>'IEA 2019 outlook'!AA5*10^3</f>
+        <v>3402145.9643264567</v>
+      </c>
+      <c r="AB7" s="17">
+        <f>'IEA 2019 outlook'!AB5*10^3</f>
+        <v>3532218.9464896857</v>
+      </c>
+      <c r="AC7" s="17">
+        <f>'IEA 2019 outlook'!AC5*10^3</f>
+        <v>3662291.9286529142</v>
+      </c>
+      <c r="AD7" s="17">
+        <f>'IEA 2019 outlook'!AD5*10^3</f>
+        <v>3792364.9108161419</v>
+      </c>
+      <c r="AE7" s="17">
+        <f>'IEA 2019 outlook'!AE5*10^3</f>
+        <v>3931484.2859526561</v>
+      </c>
+      <c r="AF7" s="17">
+        <f>'IEA 2019 outlook'!AF5*10^3</f>
+        <v>4070603.6610891712</v>
+      </c>
+      <c r="AG7" s="17">
+        <f>'IEA 2019 outlook'!AG5*10^3</f>
+        <v>4209723.0362256858</v>
+      </c>
+      <c r="AH7" s="17">
+        <f>'IEA 2019 outlook'!AH5*10^3</f>
+        <v>4348842.4113622</v>
+      </c>
+      <c r="AI7" s="17">
+        <f>'IEA 2019 outlook'!AI5*10^3</f>
+        <v>4487961.7864987161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="17">
-        <f>Solar_Capacity!G12*10^3</f>
-        <v>337846.48924046109</v>
-      </c>
-      <c r="C7" s="17">
-        <f>Solar_Capacity!H12*10^3</f>
-        <v>391129.72331994592</v>
-      </c>
-      <c r="D7" s="17">
-        <f>Solar_Capacity!I12*10^3</f>
-        <v>444412.95739943074</v>
-      </c>
-      <c r="E7" s="17">
-        <f>Solar_Capacity!J12*10^3</f>
-        <v>497696.19147891557</v>
-      </c>
-      <c r="F7" s="17">
-        <f>Solar_Capacity!K12*10^3</f>
-        <v>550979.42555840046</v>
-      </c>
-      <c r="G7" s="17">
-        <f>Solar_Capacity!L12*10^3</f>
-        <v>604262.65963788528</v>
-      </c>
-      <c r="H7" s="17">
-        <f>Solar_Capacity!M12*10^3</f>
-        <v>657545.89371737011</v>
-      </c>
-      <c r="I7" s="17">
-        <f>Solar_Capacity!N12*10^3</f>
-        <v>710829.12779685494</v>
-      </c>
-      <c r="J7" s="17">
-        <f>Solar_Capacity!O12*10^3</f>
-        <v>764112.36187634</v>
-      </c>
-      <c r="K7" s="17">
-        <f>Solar_Capacity!P12*10^3</f>
-        <v>824373.50851332222</v>
-      </c>
-      <c r="L7" s="17">
-        <f>Solar_Capacity!Q12*10^3</f>
-        <v>884634.65515030455</v>
-      </c>
-      <c r="M7" s="17">
-        <f>Solar_Capacity!R12*10^3</f>
-        <v>944895.80178728676</v>
-      </c>
-      <c r="N7" s="17">
-        <f>Solar_Capacity!S12*10^3</f>
-        <v>1005156.9484242691</v>
-      </c>
-      <c r="O7" s="17">
-        <f>Solar_Capacity!T12*10^3</f>
-        <v>1065418.0950612514</v>
-      </c>
-      <c r="P7" s="17">
-        <f>Solar_Capacity!U12*10^3</f>
-        <v>1121979.8241718928</v>
-      </c>
-      <c r="Q7" s="17">
-        <f>Solar_Capacity!V12*10^3</f>
-        <v>1178541.5532825342</v>
-      </c>
-      <c r="R7" s="17">
-        <f>Solar_Capacity!W12*10^3</f>
-        <v>1235103.2823931756</v>
-      </c>
-      <c r="S7" s="17">
-        <f>Solar_Capacity!X12*10^3</f>
-        <v>1291665.011503817</v>
-      </c>
-      <c r="T7" s="17">
-        <f>Solar_Capacity!Y12*10^3</f>
-        <v>1348226.7406144589</v>
-      </c>
-      <c r="U7" s="17">
-        <f>Solar_Capacity!Z12*10^3</f>
-        <v>1414123.5129586288</v>
-      </c>
-      <c r="V7" s="17">
-        <f>Solar_Capacity!AA12*10^3</f>
-        <v>1480020.2853027987</v>
-      </c>
-      <c r="W7" s="17">
-        <f>Solar_Capacity!AB12*10^3</f>
-        <v>1545917.0576469686</v>
-      </c>
-      <c r="X7" s="17">
-        <f>Solar_Capacity!AC12*10^3</f>
-        <v>1611813.8299911385</v>
-      </c>
-      <c r="Y7" s="17">
-        <f>Solar_Capacity!AD12*10^3</f>
-        <v>1677710.6023353089</v>
-      </c>
-      <c r="Z7" s="17">
-        <f>Solar_Capacity!AE12*10^3</f>
-        <v>1747164.7147645324</v>
-      </c>
-      <c r="AA7" s="17">
-        <f>Solar_Capacity!AF12*10^3</f>
-        <v>1816618.8271937559</v>
-      </c>
-      <c r="AB7" s="17">
-        <f>Solar_Capacity!AG12*10^3</f>
-        <v>1886072.9396229791</v>
-      </c>
-      <c r="AC7" s="17">
-        <f>Solar_Capacity!AH12*10^3</f>
-        <v>1955527.0520522026</v>
-      </c>
-      <c r="AD7" s="17">
-        <f>Solar_Capacity!AI12*10^3</f>
-        <v>2024981.1644814257</v>
-      </c>
-      <c r="AE7" s="17">
-        <f>Solar_Capacity!AJ12*10^3</f>
-        <v>2099265.7127490239</v>
-      </c>
-      <c r="AF7" s="17">
-        <f>Solar_Capacity!AK12*10^3</f>
-        <v>2173550.2610166222</v>
-      </c>
-      <c r="AG7" s="17">
-        <f>Solar_Capacity!AL12*10^3</f>
-        <v>2247834.8092842204</v>
-      </c>
-      <c r="AH7" s="17">
-        <f>Solar_Capacity!AM12*10^3</f>
-        <v>2322119.3575518192</v>
-      </c>
-      <c r="AI7" s="17">
-        <f>Solar_Capacity!AN12*10^3</f>
-        <v>2396403.9058194174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A8" s="16" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AF8">
-        <v>0</v>
-      </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A9" s="16" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9">
-        <v>0</v>
-      </c>
-      <c r="AC9">
-        <v>0</v>
-      </c>
-      <c r="AD9">
-        <v>0</v>
-      </c>
-      <c r="AE9">
-        <v>0</v>
-      </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
-      <c r="AG9">
-        <v>0</v>
-      </c>
-      <c r="AH9">
-        <v>0</v>
-      </c>
-      <c r="AI9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A10" s="16" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-      <c r="Z10">
-        <v>0</v>
-      </c>
-      <c r="AA10">
-        <v>0</v>
-      </c>
-      <c r="AB10">
-        <v>0</v>
-      </c>
-      <c r="AC10">
-        <v>0</v>
-      </c>
-      <c r="AD10">
-        <v>0</v>
-      </c>
-      <c r="AE10">
-        <v>0</v>
-      </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
-      <c r="AG10">
-        <v>0</v>
-      </c>
-      <c r="AH10">
-        <v>0</v>
-      </c>
-      <c r="AI10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A11" s="16" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <v>0</v>
-      </c>
-      <c r="AI11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A12" s="16" t="s">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
-      <c r="Z12">
-        <v>0</v>
-      </c>
-      <c r="AA12">
-        <v>0</v>
-      </c>
-      <c r="AB12">
-        <v>0</v>
-      </c>
-      <c r="AC12">
-        <v>0</v>
-      </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
-      <c r="AE12">
-        <v>0</v>
-      </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
-      <c r="AG12">
-        <v>0</v>
-      </c>
-      <c r="AH12">
-        <v>0</v>
-      </c>
-      <c r="AI12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A13" s="16" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
-      <c r="AB13">
-        <v>0</v>
-      </c>
-      <c r="AC13">
-        <v>0</v>
-      </c>
-      <c r="AD13">
-        <v>0</v>
-      </c>
-      <c r="AE13">
-        <v>0</v>
-      </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
-      <c r="AG13">
-        <v>0</v>
-      </c>
-      <c r="AH13">
-        <v>0</v>
-      </c>
-      <c r="AI13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A14" s="16" t="s">
-        <v>36</v>
-      </c>
       <c r="B14" s="17">
-        <f>Wind_Capacity!G10*10^3</f>
+        <f>'IEA 2017 Wind'!G10*10^3</f>
         <v>13143.338992959158</v>
       </c>
       <c r="C14" s="17">
-        <f>Wind_Capacity!H10*10^3</f>
+        <f>'IEA 2017 Wind'!H10*10^3</f>
         <v>14603.391990612212</v>
       </c>
       <c r="D14" s="17">
-        <f>Wind_Capacity!I10*10^3</f>
+        <f>'IEA 2017 Wind'!I10*10^3</f>
         <v>16063.444988265264</v>
       </c>
       <c r="E14" s="17">
-        <f>Wind_Capacity!J10*10^3</f>
+        <f>'IEA 2017 Wind'!J10*10^3</f>
         <v>17523.497985918319</v>
       </c>
       <c r="F14" s="17">
-        <f>Wind_Capacity!K10*10^3</f>
+        <f>'IEA 2017 Wind'!K10*10^3</f>
         <v>18983.550983571375</v>
       </c>
       <c r="G14" s="17">
-        <f>Wind_Capacity!L10*10^3</f>
+        <f>'IEA 2017 Wind'!L10*10^3</f>
         <v>20443.603981224427</v>
       </c>
       <c r="H14" s="17">
-        <f>Wind_Capacity!M10*10^3</f>
+        <f>'IEA 2017 Wind'!M10*10^3</f>
         <v>21903.656978877483</v>
       </c>
       <c r="I14" s="17">
-        <f>Wind_Capacity!N10*10^3</f>
+        <f>'IEA 2017 Wind'!N10*10^3</f>
         <v>23363.709976530536</v>
       </c>
       <c r="J14" s="17">
-        <f>Wind_Capacity!O10*10^3</f>
+        <f>'IEA 2017 Wind'!O10*10^3</f>
         <v>24823.762974183584</v>
       </c>
       <c r="K14" s="17">
-        <f>Wind_Capacity!P10*10^3</f>
+        <f>'IEA 2017 Wind'!P10*10^3</f>
         <v>27558.971215653626</v>
       </c>
       <c r="L14" s="17">
-        <f>Wind_Capacity!Q10*10^3</f>
+        <f>'IEA 2017 Wind'!Q10*10^3</f>
         <v>30294.179457123671</v>
       </c>
       <c r="M14" s="17">
-        <f>Wind_Capacity!R10*10^3</f>
+        <f>'IEA 2017 Wind'!R10*10^3</f>
         <v>33029.387698593717</v>
       </c>
       <c r="N14" s="17">
-        <f>Wind_Capacity!S10*10^3</f>
+        <f>'IEA 2017 Wind'!S10*10^3</f>
         <v>35764.595940063758</v>
       </c>
       <c r="O14" s="17">
-        <f>Wind_Capacity!T10*10^3</f>
+        <f>'IEA 2017 Wind'!T10*10^3</f>
         <v>38499.804181533807</v>
       </c>
       <c r="P14" s="17">
-        <f>Wind_Capacity!U10*10^3</f>
+        <f>'IEA 2017 Wind'!U10*10^3</f>
         <v>41725.219802228174</v>
       </c>
       <c r="Q14" s="17">
-        <f>Wind_Capacity!V10*10^3</f>
+        <f>'IEA 2017 Wind'!V10*10^3</f>
         <v>44950.635422922547</v>
       </c>
       <c r="R14" s="17">
-        <f>Wind_Capacity!W10*10^3</f>
+        <f>'IEA 2017 Wind'!W10*10^3</f>
         <v>48176.051043616913</v>
       </c>
       <c r="S14" s="17">
-        <f>Wind_Capacity!X10*10^3</f>
+        <f>'IEA 2017 Wind'!X10*10^3</f>
         <v>51401.466664311287</v>
       </c>
       <c r="T14" s="17">
-        <f>Wind_Capacity!Y10*10^3</f>
+        <f>'IEA 2017 Wind'!Y10*10^3</f>
         <v>54626.882285005646</v>
       </c>
       <c r="U14" s="17">
-        <f>Wind_Capacity!Z10*10^3</f>
+        <f>'IEA 2017 Wind'!Z10*10^3</f>
         <v>58529.875166205908</v>
       </c>
       <c r="V14" s="17">
-        <f>Wind_Capacity!AA10*10^3</f>
+        <f>'IEA 2017 Wind'!AA10*10^3</f>
         <v>62432.868047406162</v>
       </c>
       <c r="W14" s="17">
-        <f>Wind_Capacity!AB10*10^3</f>
+        <f>'IEA 2017 Wind'!AB10*10^3</f>
         <v>66335.860928606402</v>
       </c>
       <c r="X14" s="17">
-        <f>Wind_Capacity!AC10*10^3</f>
+        <f>'IEA 2017 Wind'!AC10*10^3</f>
         <v>70238.853809806649</v>
       </c>
       <c r="Y14" s="17">
-        <f>Wind_Capacity!AD10*10^3</f>
+        <f>'IEA 2017 Wind'!AD10*10^3</f>
         <v>74141.846691006926</v>
       </c>
       <c r="Z14" s="17">
-        <f>Wind_Capacity!AE10*10^3</f>
+        <f>'IEA 2017 Wind'!AE10*10^3</f>
         <v>79266.960143990786</v>
       </c>
       <c r="AA14" s="17">
-        <f>Wind_Capacity!AF10*10^3</f>
+        <f>'IEA 2017 Wind'!AF10*10^3</f>
         <v>84392.07359697466</v>
       </c>
       <c r="AB14" s="17">
-        <f>Wind_Capacity!AG10*10^3</f>
+        <f>'IEA 2017 Wind'!AG10*10^3</f>
         <v>89517.18704995852</v>
       </c>
       <c r="AC14" s="17">
-        <f>Wind_Capacity!AH10*10^3</f>
+        <f>'IEA 2017 Wind'!AH10*10^3</f>
         <v>94642.300502942395</v>
       </c>
       <c r="AD14" s="17">
-        <f>Wind_Capacity!AI10*10^3</f>
+        <f>'IEA 2017 Wind'!AI10*10^3</f>
         <v>99767.41395592624</v>
       </c>
       <c r="AE14" s="17">
-        <f>Wind_Capacity!AJ10*10^3</f>
+        <f>'IEA 2017 Wind'!AJ10*10^3</f>
         <v>106929.33781320453</v>
       </c>
       <c r="AF14" s="17">
-        <f>Wind_Capacity!AK10*10^3</f>
+        <f>'IEA 2017 Wind'!AK10*10^3</f>
         <v>114091.26167048281</v>
       </c>
       <c r="AG14" s="17">
-        <f>Wind_Capacity!AL10*10^3</f>
+        <f>'IEA 2017 Wind'!AL10*10^3</f>
         <v>121253.18552776109</v>
       </c>
       <c r="AH14" s="17">
-        <f>Wind_Capacity!AM10*10^3</f>
+        <f>'IEA 2017 Wind'!AM10*10^3</f>
         <v>128415.10938503935</v>
       </c>
       <c r="AI14" s="17">
-        <f>Wind_Capacity!AN10*10^3</f>
+        <f>'IEA 2017 Wind'!AN10*10^3</f>
         <v>135577.03324231764</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>0</v>
-      </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
-      <c r="AB15">
-        <v>0</v>
-      </c>
-      <c r="AC15">
-        <v>0</v>
-      </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
-      <c r="AE15">
-        <v>0</v>
-      </c>
-      <c r="AF15">
-        <v>0</v>
-      </c>
-      <c r="AG15">
-        <v>0</v>
-      </c>
-      <c r="AH15">
-        <v>0</v>
-      </c>
-      <c r="AI15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A16" s="12" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16">
-        <v>0</v>
-      </c>
-      <c r="X16">
-        <v>0</v>
-      </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-      <c r="Z16">
-        <v>0</v>
-      </c>
-      <c r="AA16">
-        <v>0</v>
-      </c>
-      <c r="AB16">
-        <v>0</v>
-      </c>
-      <c r="AC16">
-        <v>0</v>
-      </c>
-      <c r="AD16">
-        <v>0</v>
-      </c>
-      <c r="AE16">
-        <v>0</v>
-      </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
-      <c r="AG16">
-        <v>0</v>
-      </c>
-      <c r="AH16">
-        <v>0</v>
-      </c>
-      <c r="AI16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A17" s="12" t="s">
-        <v>44</v>
       </c>
       <c r="B17">
         <v>0</v>

</xml_diff>

<commit_message>
Update global wind and solar outlooks to use World Energy Outlook 2023
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/BGSaWC/BAU Global Solar and Wind Cap.xlsx
+++ b/InputData/endo-learn/BGSaWC/BAU Global Solar and Wind Cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\endo-learn\BGSaWC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\endo-learn\BGSaWC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C2C575-518F-4655-8799-2DDC3F3A1CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA982CF-0EBE-4F28-8898-75DEFF6B6E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>BGSaWC BAU Global Solar and Wind Capacities</t>
   </si>
@@ -137,18 +137,6 @@
     <t>Solar and Wind</t>
   </si>
   <si>
-    <t>International Renewable Energy Agency</t>
-  </si>
-  <si>
-    <t>Global Renewables Outlook</t>
-  </si>
-  <si>
-    <t>https://www.irena.org/publications/2020/Apr/Global-Renewables-Outlook-2020</t>
-  </si>
-  <si>
-    <t>Figure S.4</t>
-  </si>
-  <si>
     <t>We assume solar capacity reported be IEA is already in AC.</t>
   </si>
   <si>
@@ -198,6 +186,15 @@
   </si>
   <si>
     <t>hydrogen combined cycle</t>
+  </si>
+  <si>
+    <t>https://www.iea.org/data-and-statistics/data-product/world-energy-outlook-2023-free-dataset-2#data-files</t>
+  </si>
+  <si>
+    <t>Global Data Set</t>
+  </si>
+  <si>
+    <t>World Energy Outlook 2023 Free Dataset</t>
   </si>
 </sst>
 </file>
@@ -408,55 +405,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>532008</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>151590</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="190499" y="1819275"/>
-          <a:ext cx="11123809" cy="6476190"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1176,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,32 +1148,32 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
-        <v>2020</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1260,28 +1208,27 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1291,7 +1238,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1300,7 +1249,7 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B1">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1">
         <v>2030</v>
@@ -1311,30 +1260,30 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B2">
-        <v>582</v>
+        <v>924.78</v>
       </c>
       <c r="C2">
-        <v>2037</v>
+        <v>4698.96</v>
       </c>
       <c r="D2">
-        <v>4474</v>
+        <v>12639</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B3">
-        <v>624</v>
+        <v>827</v>
       </c>
       <c r="C3">
-        <v>1455</v>
+        <v>2064</v>
       </c>
       <c r="D3">
-        <v>2434</v>
+        <v>3874</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
@@ -1437,273 +1386,272 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6">
-        <f>TREND($B$2:$C$2,$B$1:$C$1,B5)*1000</f>
-        <v>582000</v>
+        <f t="shared" ref="B6:C6" si="0">TREND($B$2:$C$2,$B$1:$C$1,B5)*1000</f>
+        <v>86073.33333324641</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:M6" si="0">TREND($B$2:$C$2,$B$1:$C$1,C5)*1000</f>
-        <v>714272.72727276431</v>
+        <f t="shared" si="0"/>
+        <v>505426.66666663717</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>846545.45454547042</v>
+        <f>TREND($B$2:$C$2,$B$1:$C$1,D5)*1000</f>
+        <v>924779.99999991152</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>978818.18181823473</v>
+        <f t="shared" ref="E6:M6" si="1">TREND($B$2:$C$2,$B$1:$C$1,E5)*1000</f>
+        <v>1344133.3333333023</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>1111090.9090909408</v>
+        <f t="shared" si="1"/>
+        <v>1763486.6666665766</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>1243363.6363636469</v>
+        <f t="shared" si="1"/>
+        <v>2182839.9999999674</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
-        <v>1375636.3636364113</v>
+        <f t="shared" si="1"/>
+        <v>2602193.3333332418</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
-        <v>1507909.0909091174</v>
+        <f t="shared" si="1"/>
+        <v>3021546.6666666325</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1640181.8181818235</v>
+        <f t="shared" si="1"/>
+        <v>3440899.9999999069</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>1772454.5454545878</v>
+        <f t="shared" si="1"/>
+        <v>3860253.3333332976</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
-        <v>1904727.2727272939</v>
+        <f t="shared" si="1"/>
+        <v>4279606.666666572</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
-        <v>2037000</v>
+        <f t="shared" si="1"/>
+        <v>4698959.9999999627</v>
       </c>
       <c r="N6">
         <f>TREND($C$2:$D$2,$C$1:$D$1,N5)*1000</f>
-        <v>2158849.9999999767</v>
+        <v>5095961.9999999413</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:AG6" si="1">TREND($C$2:$D$2,$C$1:$D$1,O5)*1000</f>
-        <v>2280699.9999999823</v>
+        <f t="shared" ref="O6:AG6" si="2">TREND($C$2:$D$2,$C$1:$D$1,O5)*1000</f>
+        <v>5492963.9999999199</v>
       </c>
       <c r="P6">
-        <f t="shared" si="1"/>
-        <v>2402549.9999999884</v>
+        <f t="shared" si="2"/>
+        <v>5889965.9999998985</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="1"/>
-        <v>2524399.9999999944</v>
+        <f t="shared" si="2"/>
+        <v>6286967.9999998771</v>
       </c>
       <c r="R6">
-        <f t="shared" si="1"/>
-        <v>2646250</v>
+        <f t="shared" si="2"/>
+        <v>6683969.9999999721</v>
       </c>
       <c r="S6">
-        <f t="shared" si="1"/>
-        <v>2768099.9999999767</v>
+        <f t="shared" si="2"/>
+        <v>7080971.9999999506</v>
       </c>
       <c r="T6">
-        <f t="shared" si="1"/>
-        <v>2889949.9999999823</v>
+        <f t="shared" si="2"/>
+        <v>7477973.9999999292</v>
       </c>
       <c r="U6">
-        <f t="shared" si="1"/>
-        <v>3011799.9999999884</v>
+        <f t="shared" si="2"/>
+        <v>7874975.9999999078</v>
       </c>
       <c r="V6">
-        <f t="shared" si="1"/>
-        <v>3133649.9999999944</v>
+        <f t="shared" si="2"/>
+        <v>8271977.9999998864</v>
       </c>
       <c r="W6">
-        <f t="shared" si="1"/>
-        <v>3255500</v>
+        <f t="shared" si="2"/>
+        <v>8668979.9999999814</v>
       </c>
       <c r="X6">
-        <f t="shared" si="1"/>
-        <v>3377349.9999999767</v>
+        <f t="shared" si="2"/>
+        <v>9065981.999999959</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="1"/>
-        <v>3499199.9999999823</v>
+        <f t="shared" si="2"/>
+        <v>9462983.9999999385</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="1"/>
-        <v>3621049.9999999884</v>
+        <f t="shared" si="2"/>
+        <v>9859985.999999918</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="1"/>
-        <v>3742899.9999999944</v>
+        <f t="shared" si="2"/>
+        <v>10256987.999999896</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="1"/>
-        <v>3864750</v>
+        <f t="shared" si="2"/>
+        <v>10653989.999999873</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="1"/>
-        <v>3986599.9999999767</v>
+        <f t="shared" si="2"/>
+        <v>11050991.99999997</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="1"/>
-        <v>4108449.9999999823</v>
+        <f t="shared" si="2"/>
+        <v>11447993.999999948</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="1"/>
-        <v>4230299.9999999888</v>
+        <f t="shared" si="2"/>
+        <v>11844995.999999925</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="1"/>
-        <v>4352149.9999999944</v>
+        <f t="shared" si="2"/>
+        <v>12241997.999999905</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="1"/>
-        <v>4474000</v>
+        <f t="shared" si="2"/>
+        <v>12638999.999999885</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B7">
-        <f>TREND($B$3:$C$3,$B$1:$C$1,B5)*1000</f>
-        <v>624000</v>
+        <f t="shared" ref="B7:C7" si="3">TREND($B$3:$C$3,$B$1:$C$1,B5)*1000</f>
+        <v>552111.11111112405</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:M7" si="2">TREND($B$3:$C$3,$B$1:$C$1,C5)*1000</f>
-        <v>699545.45454544132</v>
+        <f t="shared" si="3"/>
+        <v>689555.55555556202</v>
       </c>
       <c r="D7">
-        <f t="shared" si="2"/>
-        <v>775090.90909091174</v>
+        <f t="shared" ref="D7:M7" si="4">TREND($B$3:$C$3,$B$1:$C$1,D5)*1000</f>
+        <v>827000</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
-        <v>850636.36363635305</v>
+        <f t="shared" si="4"/>
+        <v>964444.44444443798</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
-        <v>926181.81818182347</v>
+        <f t="shared" si="4"/>
+        <v>1101888.888888876</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
-        <v>1001727.2727272648</v>
+        <f t="shared" si="4"/>
+        <v>1239333.3333333139</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
-        <v>1077272.7272727352</v>
+        <f t="shared" si="4"/>
+        <v>1376777.7777777519</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
-        <v>1152818.1818181765</v>
+        <f t="shared" si="4"/>
+        <v>1514222.2222222481</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
-        <v>1228363.6363636178</v>
+        <f t="shared" si="4"/>
+        <v>1651666.6666666861</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
-        <v>1303909.0909090883</v>
+        <f t="shared" si="4"/>
+        <v>1789111.111111124</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
-        <v>1379454.5454545296</v>
+        <f t="shared" si="4"/>
+        <v>1926555.555555562</v>
       </c>
       <c r="M7">
-        <f t="shared" si="2"/>
-        <v>1455000</v>
+        <f t="shared" si="4"/>
+        <v>2064000</v>
       </c>
       <c r="N7">
         <f>TREND($C$3:$D$3,$C$1:$D$1,N5)*1000</f>
-        <v>1503950.0000000116</v>
+        <v>2154500</v>
       </c>
       <c r="O7">
-        <f t="shared" ref="O7:AG7" si="3">TREND($C$3:$D$3,$C$1:$D$1,O5)*1000</f>
-        <v>1552900.0000000088</v>
+        <f t="shared" ref="O7:AG7" si="5">TREND($C$3:$D$3,$C$1:$D$1,O5)*1000</f>
+        <v>2245000</v>
       </c>
       <c r="P7">
-        <f t="shared" si="3"/>
-        <v>1601850.0000000058</v>
+        <f t="shared" si="5"/>
+        <v>2335500</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="3"/>
-        <v>1650800.0000000028</v>
+        <f t="shared" si="5"/>
+        <v>2426000</v>
       </c>
       <c r="R7">
-        <f t="shared" si="3"/>
-        <v>1699750</v>
+        <f t="shared" si="5"/>
+        <v>2516500</v>
       </c>
       <c r="S7">
-        <f t="shared" si="3"/>
-        <v>1748700.0000000116</v>
+        <f t="shared" si="5"/>
+        <v>2607000</v>
       </c>
       <c r="T7">
-        <f t="shared" si="3"/>
-        <v>1797650.0000000088</v>
+        <f t="shared" si="5"/>
+        <v>2697500</v>
       </c>
       <c r="U7">
-        <f t="shared" si="3"/>
-        <v>1846600.0000000058</v>
+        <f t="shared" si="5"/>
+        <v>2788000</v>
       </c>
       <c r="V7">
-        <f t="shared" si="3"/>
-        <v>1895550.0000000028</v>
+        <f t="shared" si="5"/>
+        <v>2878500</v>
       </c>
       <c r="W7">
-        <f t="shared" si="3"/>
-        <v>1944500</v>
+        <f t="shared" si="5"/>
+        <v>2969000</v>
       </c>
       <c r="X7">
-        <f t="shared" si="3"/>
-        <v>1993450.0000000116</v>
+        <f t="shared" si="5"/>
+        <v>3059500</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="3"/>
-        <v>2042400.0000000088</v>
+        <f t="shared" si="5"/>
+        <v>3150000</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="3"/>
-        <v>2091350.0000000058</v>
+        <f t="shared" si="5"/>
+        <v>3240500</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="3"/>
-        <v>2140300.0000000028</v>
+        <f t="shared" si="5"/>
+        <v>3331000</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="3"/>
-        <v>2189250</v>
+        <f t="shared" si="5"/>
+        <v>3421500</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="3"/>
-        <v>2238200.0000000116</v>
+        <f t="shared" si="5"/>
+        <v>3512000</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="3"/>
-        <v>2287150.0000000088</v>
+        <f t="shared" si="5"/>
+        <v>3602500</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="3"/>
-        <v>2336100.0000000056</v>
+        <f t="shared" si="5"/>
+        <v>3693000</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="3"/>
-        <v>2385050.0000000028</v>
+        <f t="shared" si="5"/>
+        <v>3783500</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="3"/>
-        <v>2434000</v>
+        <f t="shared" si="5"/>
+        <v>3874000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2143,7 +2091,7 @@
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <f>D10/D9</f>
@@ -2596,7 +2544,7 @@
   </sheetPr>
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -2623,7 +2571,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2631,7 +2579,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2659,7 +2607,7 @@
       </c>
       <c r="B7" s="14">
         <f>'Global Renewables Outlook'!C7*(1-'IEA 2017 Wind'!J12)</f>
-        <v>681371.59811876004</v>
+        <v>671641.2319280426</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2698,7 +2646,7 @@
       </c>
       <c r="B8" s="14">
         <f>'Global Renewables Outlook'!C6</f>
-        <v>714272.72727276431</v>
+        <v>505426.66666663717</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -2785,7 +2733,7 @@
       </c>
       <c r="B15" s="14">
         <f>'Global Renewables Outlook'!C7*'IEA 2017 Wind'!J12</f>
-        <v>18173.856426681279</v>
+        <v>17914.323627519447</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -2844,7 +2792,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2852,7 +2800,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -2860,7 +2808,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -2868,7 +2816,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -2876,7 +2824,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -2884,7 +2832,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -2892,7 +2840,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -3111,7 +3059,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3206,7 +3154,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -3495,123 +3443,123 @@
       </c>
       <c r="B7" s="14">
         <f>'Global Renewables Outlook'!D7*(1-'IEA 2017 Wind'!K12)</f>
-        <v>754938.35798369965</v>
+        <v>805497.79997392592</v>
       </c>
       <c r="C7" s="14">
         <f>'Global Renewables Outlook'!E7*(1-'IEA 2017 Wind'!L12)</f>
-        <v>828504.48238323536</v>
+        <v>939351.50128782692</v>
       </c>
       <c r="D7" s="14">
         <f>'Global Renewables Outlook'!F7*(1-'IEA 2017 Wind'!M12)</f>
-        <v>902070.09733831172</v>
+        <v>1073202.9043792556</v>
       </c>
       <c r="E7" s="14">
         <f>'Global Renewables Outlook'!G7*(1-'IEA 2017 Wind'!N12)</f>
-        <v>975635.29761384299</v>
+        <v>1207052.4367550183</v>
       </c>
       <c r="F7" s="14">
         <f>'Global Renewables Outlook'!H7*(1-'IEA 2017 Wind'!O12)</f>
-        <v>1049200.1558433597</v>
+        <v>1340900.4260815941</v>
       </c>
       <c r="G7" s="14">
         <f>'Global Renewables Outlook'!I7*(1-'IEA 2017 Wind'!P12)</f>
-        <v>1121222.8094770459</v>
+        <v>1472721.822876645</v>
       </c>
       <c r="H7" s="14">
         <f>'Global Renewables Outlook'!J7*(1-'IEA 2017 Wind'!Q12)</f>
-        <v>1193207.4250556889</v>
+        <v>1604395.369613728</v>
       </c>
       <c r="I7" s="14">
         <f>'Global Renewables Outlook'!K7*(1-'IEA 2017 Wind'!R12)</f>
-        <v>1265159.4382497929</v>
+        <v>1735942.1941921487</v>
       </c>
       <c r="J7" s="14">
         <f>'Global Renewables Outlook'!L7*(1-'IEA 2017 Wind'!S12)</f>
-        <v>1337083.296137417</v>
+        <v>1867379.5819530278</v>
       </c>
       <c r="K7" s="14">
         <f>'Global Renewables Outlook'!M7*(1-'IEA 2017 Wind'!T12)</f>
-        <v>1408982.6721757923</v>
+        <v>1998721.8112514331</v>
       </c>
       <c r="L7" s="14">
         <f>'Global Renewables Outlook'!N7*(1-'IEA 2017 Wind'!U12)</f>
-        <v>1454354.0181945674</v>
+        <v>2083450.734532512</v>
       </c>
       <c r="M7" s="14">
         <f>'Global Renewables Outlook'!O7*(1-'IEA 2017 Wind'!V12)</f>
-        <v>1499746.3552090656</v>
+        <v>2168156.7180400109</v>
       </c>
       <c r="N7" s="14">
         <f>'Global Renewables Outlook'!P7*(1-'IEA 2017 Wind'!W12)</f>
-        <v>1545157.4640270318</v>
+        <v>2252842.186993239</v>
       </c>
       <c r="O7" s="14">
         <f>'Global Renewables Outlook'!Q7*(1-'IEA 2017 Wind'!X12)</f>
-        <v>1590585.4276282906</v>
+        <v>2337509.2363861315</v>
       </c>
       <c r="P7" s="14">
         <f>'Global Renewables Outlook'!R7*(1-'IEA 2017 Wind'!Y12)</f>
-        <v>1636028.58142701</v>
+        <v>2422159.6853425922</v>
       </c>
       <c r="Q7" s="14">
         <f>'Global Renewables Outlook'!S7*(1-'IEA 2017 Wind'!Z12)</f>
-        <v>1680197.7520111771</v>
+        <v>2504875.3585481266</v>
       </c>
       <c r="R7" s="14">
         <f>'Global Renewables Outlook'!T7*(1-'IEA 2017 Wind'!AA12)</f>
-        <v>1724348.2566176786</v>
+        <v>2587505.5890891803</v>
       </c>
       <c r="S7" s="14">
         <f>'Global Renewables Outlook'!U7*(1-'IEA 2017 Wind'!AB12)</f>
-        <v>1768481.4155999315</v>
+        <v>2670056.4208234558</v>
       </c>
       <c r="T7" s="14">
         <f>'Global Renewables Outlook'!V7*(1-'IEA 2017 Wind'!AC12)</f>
-        <v>1812598.4276515185</v>
+        <v>2752533.3407163559</v>
       </c>
       <c r="U7" s="14">
         <f>'Global Renewables Outlook'!W7*(1-'IEA 2017 Wind'!AD12)</f>
-        <v>1856700.3835031393</v>
+        <v>2834941.3415380921</v>
       </c>
       <c r="V7" s="14">
         <f>'Global Renewables Outlook'!X7*(1-'IEA 2017 Wind'!AE12)</f>
-        <v>1899173.3917596261</v>
+        <v>2914806.4872901463</v>
       </c>
       <c r="W7" s="14">
         <f>'Global Renewables Outlook'!Y7*(1-'IEA 2017 Wind'!AF12)</f>
-        <v>1941610.9600069062</v>
+        <v>2994552.7438414255</v>
       </c>
       <c r="X7" s="14">
         <f>'Global Renewables Outlook'!Z7*(1-'IEA 2017 Wind'!AG12)</f>
-        <v>1984015.1641012894</v>
+        <v>3074187.0749851582</v>
       </c>
       <c r="Y7" s="14">
         <f>'Global Renewables Outlook'!AA7*(1-'IEA 2017 Wind'!AH12)</f>
-        <v>2026387.9208827256</v>
+        <v>3153715.9110687054</v>
       </c>
       <c r="Z7" s="14">
         <f>'Global Renewables Outlook'!AB7*(1-'IEA 2017 Wind'!AI12)</f>
-        <v>2068731.0031150684</v>
+        <v>3233145.1991130328</v>
       </c>
       <c r="AA7" s="14">
         <f>'Global Renewables Outlook'!AC7*(1-'IEA 2017 Wind'!AJ12)</f>
-        <v>2109832.2301834417</v>
+        <v>3310575.8164615356</v>
       </c>
       <c r="AB7" s="14">
         <f>'Global Renewables Outlook'!AD7*(1-'IEA 2017 Wind'!AK12)</f>
-        <v>2150994.4197746827</v>
+        <v>3388040.7481967793</v>
       </c>
       <c r="AC7" s="14">
         <f>'Global Renewables Outlook'!AE7*(1-'IEA 2017 Wind'!AL12)</f>
-        <v>2192212.7308672476</v>
+        <v>3465537.2694202843</v>
       </c>
       <c r="AD7" s="14">
         <f>'Global Renewables Outlook'!AF7*(1-'IEA 2017 Wind'!AM12)</f>
-        <v>2233482.8217879166</v>
+        <v>3543062.9363051392</v>
       </c>
       <c r="AE7" s="14">
         <f>'Global Renewables Outlook'!AG7*(1-'IEA 2017 Wind'!AN12)</f>
-        <v>2274800.7874460295</v>
+        <v>3620615.5507666054</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -3620,123 +3568,123 @@
       </c>
       <c r="B8" s="14">
         <f>'Global Renewables Outlook'!D6</f>
-        <v>846545.45454547042</v>
+        <v>924779.99999991152</v>
       </c>
       <c r="C8" s="14">
         <f>'Global Renewables Outlook'!E6</f>
-        <v>978818.18181823473</v>
+        <v>1344133.3333333023</v>
       </c>
       <c r="D8" s="14">
         <f>'Global Renewables Outlook'!F6</f>
-        <v>1111090.9090909408</v>
+        <v>1763486.6666665766</v>
       </c>
       <c r="E8" s="14">
         <f>'Global Renewables Outlook'!G6</f>
-        <v>1243363.6363636469</v>
+        <v>2182839.9999999674</v>
       </c>
       <c r="F8" s="14">
         <f>'Global Renewables Outlook'!H6</f>
-        <v>1375636.3636364113</v>
+        <v>2602193.3333332418</v>
       </c>
       <c r="G8" s="14">
         <f>'Global Renewables Outlook'!I6</f>
-        <v>1507909.0909091174</v>
+        <v>3021546.6666666325</v>
       </c>
       <c r="H8" s="14">
         <f>'Global Renewables Outlook'!J6</f>
-        <v>1640181.8181818235</v>
+        <v>3440899.9999999069</v>
       </c>
       <c r="I8" s="14">
         <f>'Global Renewables Outlook'!K6</f>
-        <v>1772454.5454545878</v>
+        <v>3860253.3333332976</v>
       </c>
       <c r="J8" s="14">
         <f>'Global Renewables Outlook'!L6</f>
-        <v>1904727.2727272939</v>
+        <v>4279606.666666572</v>
       </c>
       <c r="K8" s="14">
         <f>'Global Renewables Outlook'!M6</f>
-        <v>2037000</v>
+        <v>4698959.9999999627</v>
       </c>
       <c r="L8" s="14">
         <f>'Global Renewables Outlook'!N6</f>
-        <v>2158849.9999999767</v>
+        <v>5095961.9999999413</v>
       </c>
       <c r="M8" s="14">
         <f>'Global Renewables Outlook'!O6</f>
-        <v>2280699.9999999823</v>
+        <v>5492963.9999999199</v>
       </c>
       <c r="N8" s="14">
         <f>'Global Renewables Outlook'!P6</f>
-        <v>2402549.9999999884</v>
+        <v>5889965.9999998985</v>
       </c>
       <c r="O8" s="14">
         <f>'Global Renewables Outlook'!Q6</f>
-        <v>2524399.9999999944</v>
+        <v>6286967.9999998771</v>
       </c>
       <c r="P8" s="14">
         <f>'Global Renewables Outlook'!R6</f>
-        <v>2646250</v>
+        <v>6683969.9999999721</v>
       </c>
       <c r="Q8" s="14">
         <f>'Global Renewables Outlook'!S6</f>
-        <v>2768099.9999999767</v>
+        <v>7080971.9999999506</v>
       </c>
       <c r="R8" s="14">
         <f>'Global Renewables Outlook'!T6</f>
-        <v>2889949.9999999823</v>
+        <v>7477973.9999999292</v>
       </c>
       <c r="S8" s="14">
         <f>'Global Renewables Outlook'!U6</f>
-        <v>3011799.9999999884</v>
+        <v>7874975.9999999078</v>
       </c>
       <c r="T8" s="14">
         <f>'Global Renewables Outlook'!V6</f>
-        <v>3133649.9999999944</v>
+        <v>8271977.9999998864</v>
       </c>
       <c r="U8" s="14">
         <f>'Global Renewables Outlook'!W6</f>
-        <v>3255500</v>
+        <v>8668979.9999999814</v>
       </c>
       <c r="V8" s="14">
         <f>'Global Renewables Outlook'!X6</f>
-        <v>3377349.9999999767</v>
+        <v>9065981.999999959</v>
       </c>
       <c r="W8" s="14">
         <f>'Global Renewables Outlook'!Y6</f>
-        <v>3499199.9999999823</v>
+        <v>9462983.9999999385</v>
       </c>
       <c r="X8" s="14">
         <f>'Global Renewables Outlook'!Z6</f>
-        <v>3621049.9999999884</v>
+        <v>9859985.999999918</v>
       </c>
       <c r="Y8" s="14">
         <f>'Global Renewables Outlook'!AA6</f>
-        <v>3742899.9999999944</v>
+        <v>10256987.999999896</v>
       </c>
       <c r="Z8" s="14">
         <f>'Global Renewables Outlook'!AB6</f>
-        <v>3864750</v>
+        <v>10653989.999999873</v>
       </c>
       <c r="AA8" s="14">
         <f>'Global Renewables Outlook'!AC6</f>
-        <v>3986599.9999999767</v>
+        <v>11050991.99999997</v>
       </c>
       <c r="AB8" s="14">
         <f>'Global Renewables Outlook'!AD6</f>
-        <v>4108449.9999999823</v>
+        <v>11447993.999999948</v>
       </c>
       <c r="AC8" s="14">
         <f>'Global Renewables Outlook'!AE6</f>
-        <v>4230299.9999999888</v>
+        <v>11844995.999999925</v>
       </c>
       <c r="AD8" s="14">
         <f>'Global Renewables Outlook'!AF6</f>
-        <v>4352149.9999999944</v>
+        <v>12241997.999999905</v>
       </c>
       <c r="AE8" s="14">
         <f>'Global Renewables Outlook'!AG6</f>
-        <v>4474000</v>
+        <v>12638999.999999885</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -4315,123 +4263,123 @@
       </c>
       <c r="B15" s="14">
         <f>'Global Renewables Outlook'!D7*'IEA 2017 Wind'!K12</f>
-        <v>20152.551107212112</v>
+        <v>21502.200026074122</v>
       </c>
       <c r="C15" s="14">
         <f>'Global Renewables Outlook'!E7*'IEA 2017 Wind'!L12</f>
-        <v>22131.881253117648</v>
+        <v>25092.943156611036</v>
       </c>
       <c r="D15" s="14">
         <f>'Global Renewables Outlook'!F7*'IEA 2017 Wind'!M12</f>
-        <v>24111.720843511761</v>
+        <v>28685.984509620484</v>
       </c>
       <c r="E15" s="14">
         <f>'Global Renewables Outlook'!G7*'IEA 2017 Wind'!N12</f>
-        <v>26091.975113421791</v>
+        <v>32280.896578295553</v>
       </c>
       <c r="F15" s="14">
         <f>'Global Renewables Outlook'!H7*'IEA 2017 Wind'!O12</f>
-        <v>28072.571429375646</v>
+        <v>35877.351696157806</v>
       </c>
       <c r="G15" s="14">
         <f>'Global Renewables Outlook'!I7*'IEA 2017 Wind'!P12</f>
-        <v>31595.372341130736</v>
+        <v>41500.399345603037</v>
       </c>
       <c r="H15" s="14">
         <f>'Global Renewables Outlook'!J7*'IEA 2017 Wind'!Q12</f>
-        <v>35156.211307928854</v>
+        <v>47271.297052958194</v>
       </c>
       <c r="I15" s="14">
         <f>'Global Renewables Outlook'!K7*'IEA 2017 Wind'!R12</f>
-        <v>38749.652659295331</v>
+        <v>53168.916918975345</v>
       </c>
       <c r="J15" s="14">
         <f>'Global Renewables Outlook'!L7*'IEA 2017 Wind'!S12</f>
-        <v>42371.249317112568</v>
+        <v>59175.973602534184</v>
       </c>
       <c r="K15" s="14">
         <f>'Global Renewables Outlook'!M7*'IEA 2017 Wind'!T12</f>
-        <v>46017.327824207787</v>
+        <v>65278.188748566921</v>
       </c>
       <c r="L15" s="14">
         <f>'Global Renewables Outlook'!N7*'IEA 2017 Wind'!U12</f>
-        <v>49595.981805444135</v>
+        <v>71049.265467487989</v>
       </c>
       <c r="M15" s="14">
         <f>'Global Renewables Outlook'!O7*'IEA 2017 Wind'!V12</f>
-        <v>53153.644790943217</v>
+        <v>76843.281959988948</v>
       </c>
       <c r="N15" s="14">
         <f>'Global Renewables Outlook'!P7*'IEA 2017 Wind'!W12</f>
-        <v>56692.535972973987</v>
+        <v>82657.813006761105</v>
       </c>
       <c r="O15" s="14">
         <f>'Global Renewables Outlook'!Q7*'IEA 2017 Wind'!X12</f>
-        <v>60214.572371712304</v>
+        <v>88490.763613868316</v>
       </c>
       <c r="P15" s="14">
         <f>'Global Renewables Outlook'!R7*'IEA 2017 Wind'!Y12</f>
-        <v>63721.418572989911</v>
+        <v>94340.314657407929</v>
       </c>
       <c r="Q15" s="14">
         <f>'Global Renewables Outlook'!S7*'IEA 2017 Wind'!Z12</f>
-        <v>68502.247988834672</v>
+        <v>102124.64145187329</v>
       </c>
       <c r="R15" s="14">
         <f>'Global Renewables Outlook'!T7*'IEA 2017 Wind'!AA12</f>
-        <v>73301.743382330329</v>
+        <v>109994.41091081973</v>
       </c>
       <c r="S15" s="14">
         <f>'Global Renewables Outlook'!U7*'IEA 2017 Wind'!AB12</f>
-        <v>78118.584400074353</v>
+        <v>117943.57917654426</v>
       </c>
       <c r="T15" s="14">
         <f>'Global Renewables Outlook'!V7*'IEA 2017 Wind'!AC12</f>
-        <v>82951.572348484304</v>
+        <v>125966.65928364419</v>
       </c>
       <c r="U15" s="14">
         <f>'Global Renewables Outlook'!W7*'IEA 2017 Wind'!AD12</f>
-        <v>87799.616496860792</v>
+        <v>134058.65846190779</v>
       </c>
       <c r="V15" s="14">
         <f>'Global Renewables Outlook'!X7*'IEA 2017 Wind'!AE12</f>
-        <v>94276.608240385627</v>
+        <v>144693.51270985385</v>
       </c>
       <c r="W15" s="14">
         <f>'Global Renewables Outlook'!Y7*'IEA 2017 Wind'!AF12</f>
-        <v>100789.03999310276</v>
+        <v>155447.2561585744</v>
       </c>
       <c r="X15" s="14">
         <f>'Global Renewables Outlook'!Z7*'IEA 2017 Wind'!AG12</f>
-        <v>107334.83589871647</v>
+        <v>166312.92501484195</v>
       </c>
       <c r="Y15" s="14">
         <f>'Global Renewables Outlook'!AA7*'IEA 2017 Wind'!AH12</f>
-        <v>113912.07911727707</v>
+        <v>177284.08893129442</v>
       </c>
       <c r="Z15" s="14">
         <f>'Global Renewables Outlook'!AB7*'IEA 2017 Wind'!AI12</f>
-        <v>120518.99688493161</v>
+        <v>188354.80088696745</v>
       </c>
       <c r="AA15" s="14">
         <f>'Global Renewables Outlook'!AC7*'IEA 2017 Wind'!AJ12</f>
-        <v>128367.76981657001</v>
+        <v>201424.18353846463</v>
       </c>
       <c r="AB15" s="14">
         <f>'Global Renewables Outlook'!AD7*'IEA 2017 Wind'!AK12</f>
-        <v>136155.58022532647</v>
+        <v>214459.25180322089</v>
       </c>
       <c r="AC15" s="14">
         <f>'Global Renewables Outlook'!AE7*'IEA 2017 Wind'!AL12</f>
-        <v>143887.26913275797</v>
+        <v>227462.73057971572</v>
       </c>
       <c r="AD15" s="14">
         <f>'Global Renewables Outlook'!AF7*'IEA 2017 Wind'!AM12</f>
-        <v>151567.17821208638</v>
+        <v>240437.06369486096</v>
       </c>
       <c r="AE15" s="14">
         <f>'Global Renewables Outlook'!AG7*'IEA 2017 Wind'!AN12</f>
-        <v>159199.21255397078</v>
+        <v>253384.44923339473</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -4721,7 +4669,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -4816,7 +4764,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -4911,7 +4859,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -5006,7 +4954,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -5101,7 +5049,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -5196,7 +5144,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -5291,7 +5239,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B25">
         <v>0</v>

</xml_diff>